<commit_message>
ESN With 3 variable
</commit_message>
<xml_diff>
--- a/esn1.xlsx
+++ b/esn1.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Lan Height</t>
   </si>
   <si>
     <t>V of Oxy</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
   <si>
     <t>dc/dt</t>
@@ -78,7 +81,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -88,6 +91,9 @@
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -397,18 +403,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F145"/>
+  <dimension ref="A1:G145"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -418,14 +425,17 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="3">
@@ -434,14 +444,17 @@
       <c r="B2" s="3">
         <v>35263.453125</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
         <v>0.08776169221107463</v>
       </c>
-      <c r="D2" s="3">
+      <c r="E2" s="3">
         <v>0.186547733543836</v>
       </c>
-      <c r="E2" s="2"/>
       <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="3">
@@ -450,14 +463,17 @@
       <c r="B3" s="3">
         <v>37824.0859375</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3">
         <v>0.08178479762855982</v>
       </c>
-      <c r="D3" s="3">
+      <c r="E3" s="3">
         <v>0.184381263444471</v>
       </c>
-      <c r="E3" s="2"/>
       <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="3">
@@ -466,14 +482,17 @@
       <c r="B4" s="3">
         <v>35862.8125</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3">
         <v>0.0886620375556337</v>
       </c>
-      <c r="D4" s="3">
+      <c r="E4" s="3">
         <v>0.216999998097611</v>
       </c>
-      <c r="E4" s="2"/>
       <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="3">
@@ -482,14 +501,17 @@
       <c r="B5" s="3">
         <v>35688.8359375</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3">
         <v>0.108433518688308</v>
       </c>
-      <c r="D5" s="3">
+      <c r="E5" s="3">
         <v>0.180361980355918</v>
       </c>
-      <c r="E5" s="2"/>
       <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="3">
@@ -498,14 +520,17 @@
       <c r="B6" s="3">
         <v>35786.953125</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3">
         <v>0.10708684551010435</v>
       </c>
-      <c r="D6" s="3">
+      <c r="E6" s="3">
         <v>0.170502124052733</v>
       </c>
-      <c r="E6" s="2"/>
       <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="3">
@@ -514,14 +539,17 @@
       <c r="B7" s="3">
         <v>36151.8828125</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="4">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3">
         <v>0.11460736023016982</v>
       </c>
-      <c r="D7" s="3">
+      <c r="E7" s="3">
         <v>0.14325039144338</v>
       </c>
-      <c r="E7" s="2"/>
       <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="3">
@@ -530,14 +558,17 @@
       <c r="B8" s="3">
         <v>35690.765625</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="4">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3">
         <v>0.12335532111456833</v>
       </c>
-      <c r="D8" s="3">
+      <c r="E8" s="3">
         <v>0.0915730233373495</v>
       </c>
-      <c r="E8" s="2"/>
       <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="3">
@@ -546,15 +577,16 @@
       <c r="B9" s="3">
         <v>36317.95703125</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2"/>
+      <c r="D9" s="3">
         <v>0.12626774634817292</v>
       </c>
-      <c r="D9" s="3">
+      <c r="E9" s="3">
         <v>0.115093637774837</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2" t="s">
-        <v>4</v>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
@@ -564,14 +596,15 @@
       <c r="B10" s="3">
         <v>36020.4375</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2"/>
+      <c r="D10" s="3">
         <v>0.1308342213459785</v>
       </c>
-      <c r="D10" s="3">
+      <c r="E10" s="3">
         <v>0.132753500178766</v>
       </c>
-      <c r="E10" s="2"/>
       <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="3">
@@ -580,14 +613,15 @@
       <c r="B11" s="3">
         <v>35949.24609375</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2"/>
+      <c r="D11" s="3">
         <v>0.12683833141111628</v>
       </c>
-      <c r="D11" s="3">
+      <c r="E11" s="3">
         <v>0.137659081024871</v>
       </c>
-      <c r="E11" s="2"/>
       <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="3">
@@ -596,14 +630,15 @@
       <c r="B12" s="3">
         <v>35984.68359375</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2"/>
+      <c r="D12" s="3">
         <v>0.1258809977272501</v>
       </c>
-      <c r="D12" s="3">
+      <c r="E12" s="3">
         <v>0.136544230874021</v>
       </c>
-      <c r="E12" s="2"/>
       <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="3">
@@ -612,14 +647,15 @@
       <c r="B13" s="3">
         <v>36185.3828125</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2"/>
+      <c r="D13" s="3">
         <v>0.12709374194159173</v>
       </c>
-      <c r="D13" s="3">
+      <c r="E13" s="3">
         <v>0.160509394769273</v>
       </c>
-      <c r="E13" s="2"/>
       <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="3">
@@ -628,14 +664,15 @@
       <c r="B14" s="3">
         <v>35754.19921875</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2"/>
+      <c r="D14" s="3">
         <v>0.12633634812312242</v>
       </c>
-      <c r="D14" s="3">
+      <c r="E14" s="3">
         <v>0.120230747486478</v>
       </c>
-      <c r="E14" s="2"/>
       <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="3">
@@ -644,14 +681,15 @@
       <c r="B15" s="3">
         <v>35803.76171875</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2"/>
+      <c r="D15" s="3">
         <v>0.1287496825253159</v>
       </c>
-      <c r="D15" s="3">
+      <c r="E15" s="3">
         <v>0.140745369153456</v>
       </c>
-      <c r="E15" s="2"/>
       <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="3">
@@ -660,14 +698,15 @@
       <c r="B16" s="3">
         <v>36178.8125</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2"/>
+      <c r="D16" s="3">
         <v>0.12921883348244653</v>
       </c>
-      <c r="D16" s="3">
+      <c r="E16" s="3">
         <v>0.114961554501071</v>
       </c>
-      <c r="E16" s="2"/>
       <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="3">
@@ -676,14 +715,15 @@
       <c r="B17" s="3">
         <v>35825.9140625</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2"/>
+      <c r="D17" s="3">
         <v>0.13336369031383674</v>
       </c>
-      <c r="D17" s="3">
+      <c r="E17" s="3">
         <v>0.137229572689584</v>
       </c>
-      <c r="E17" s="2"/>
       <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="3">
@@ -692,14 +732,15 @@
       <c r="B18" s="3">
         <v>36137.8046875</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2"/>
+      <c r="D18" s="3">
         <v>0.13675216427363837</v>
       </c>
-      <c r="D18" s="3">
+      <c r="E18" s="3">
         <v>0.156145346307745</v>
       </c>
-      <c r="E18" s="2"/>
       <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="3">
@@ -708,14 +749,15 @@
       <c r="B19" s="3">
         <v>35894.79296875</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2"/>
+      <c r="D19" s="3">
         <v>0.12817431786507225</v>
       </c>
-      <c r="D19" s="3">
+      <c r="E19" s="3">
         <v>0.143516117377811</v>
       </c>
-      <c r="E19" s="2"/>
       <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="3">
@@ -724,14 +766,15 @@
       <c r="B20" s="3">
         <v>36322.484375</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2"/>
+      <c r="D20" s="3">
         <v>0.1306265153250736</v>
       </c>
-      <c r="D20" s="3">
+      <c r="E20" s="3">
         <v>0.138856279931572</v>
       </c>
-      <c r="E20" s="2"/>
       <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="3">
@@ -740,14 +783,15 @@
       <c r="B21" s="3">
         <v>35816.94921875</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="2"/>
+      <c r="D21" s="3">
         <v>0.1306625522687812</v>
       </c>
-      <c r="D21" s="3">
+      <c r="E21" s="3">
         <v>0.141604922022545</v>
       </c>
-      <c r="E21" s="2"/>
       <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="3">
@@ -756,14 +800,15 @@
       <c r="B22" s="3">
         <v>36103.69140625</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="2"/>
+      <c r="D22" s="3">
         <v>0.13295394318868056</v>
       </c>
-      <c r="D22" s="3">
+      <c r="E22" s="3">
         <v>0.144650506621306</v>
       </c>
-      <c r="E22" s="2"/>
       <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="3">
@@ -772,14 +817,15 @@
       <c r="B23" s="3">
         <v>36120.0234375</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="2"/>
+      <c r="D23" s="3">
         <v>0.133393013951299</v>
       </c>
-      <c r="D23" s="3">
+      <c r="E23" s="3">
         <v>0.132658936459608</v>
       </c>
-      <c r="E23" s="2"/>
       <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="3">
@@ -788,14 +834,15 @@
       <c r="B24" s="3">
         <v>36048.4140625</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="2"/>
+      <c r="D24" s="3">
         <v>0.1338479340939112</v>
       </c>
-      <c r="D24" s="3">
+      <c r="E24" s="3">
         <v>0.142672072871166</v>
       </c>
-      <c r="E24" s="2"/>
       <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="3">
@@ -804,14 +851,15 @@
       <c r="B25" s="3">
         <v>35934.20703125</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="2"/>
+      <c r="D25" s="3">
         <v>0.13809271968198716</v>
       </c>
-      <c r="D25" s="3">
+      <c r="E25" s="3">
         <v>0.140576922938218</v>
       </c>
-      <c r="E25" s="2"/>
       <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="3">
@@ -820,14 +868,15 @@
       <c r="B26" s="3">
         <v>35949.97265625</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="2"/>
+      <c r="D26" s="3">
         <v>0.13778955042610638</v>
       </c>
-      <c r="D26" s="3">
+      <c r="E26" s="3">
         <v>0.143467876456453</v>
       </c>
-      <c r="E26" s="2"/>
       <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="3">
@@ -836,14 +885,15 @@
       <c r="B27" s="3">
         <v>35917.9921875</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="2"/>
+      <c r="D27" s="3">
         <v>0.1411088369930353</v>
       </c>
-      <c r="D27" s="3">
+      <c r="E27" s="3">
         <v>0.142682211185802</v>
       </c>
-      <c r="E27" s="2"/>
       <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="3">
@@ -852,14 +902,15 @@
       <c r="B28" s="3">
         <v>35918.1796875</v>
       </c>
-      <c r="C28" s="3">
+      <c r="C28" s="2"/>
+      <c r="D28" s="3">
         <v>0.1456212133165516</v>
       </c>
-      <c r="D28" s="3">
+      <c r="E28" s="3">
         <v>0.139495586895171</v>
       </c>
-      <c r="E28" s="2"/>
       <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="3">
@@ -868,14 +919,15 @@
       <c r="B29" s="3">
         <v>36141.921875</v>
       </c>
-      <c r="C29" s="3">
+      <c r="C29" s="2"/>
+      <c r="D29" s="3">
         <v>0.14994183274388587</v>
       </c>
-      <c r="D29" s="3">
+      <c r="E29" s="3">
         <v>0.137079323697947</v>
       </c>
-      <c r="E29" s="2"/>
       <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="3">
@@ -884,14 +936,15 @@
       <c r="B30" s="3">
         <v>36155.109375</v>
       </c>
-      <c r="C30" s="3">
+      <c r="C30" s="2"/>
+      <c r="D30" s="3">
         <v>0.1493221710566279</v>
       </c>
-      <c r="D30" s="3">
+      <c r="E30" s="3">
         <v>0.137175087396393</v>
       </c>
-      <c r="E30" s="2"/>
       <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="3">
@@ -900,14 +953,15 @@
       <c r="B31" s="3">
         <v>36098.41796875</v>
       </c>
-      <c r="C31" s="3">
+      <c r="C31" s="2"/>
+      <c r="D31" s="3">
         <v>0.1446909481925624</v>
       </c>
-      <c r="D31" s="3">
+      <c r="E31" s="3">
         <v>0.137508033153914</v>
       </c>
-      <c r="E31" s="2"/>
       <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="3">
@@ -916,14 +970,15 @@
       <c r="B32" s="3">
         <v>36370.28515625</v>
       </c>
-      <c r="C32" s="3">
+      <c r="C32" s="2"/>
+      <c r="D32" s="3">
         <v>0.13261509364253396</v>
       </c>
-      <c r="D32" s="3">
+      <c r="E32" s="3">
         <v>0.136949985366796</v>
       </c>
-      <c r="E32" s="2"/>
       <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="3">
@@ -932,14 +987,15 @@
       <c r="B33" s="3">
         <v>35754.07421875</v>
       </c>
-      <c r="C33" s="3">
+      <c r="C33" s="2"/>
+      <c r="D33" s="3">
         <v>0.12313393213401044</v>
       </c>
-      <c r="D33" s="3">
+      <c r="E33" s="3">
         <v>0.141395679754752</v>
       </c>
-      <c r="E33" s="2"/>
       <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="3">
@@ -948,14 +1004,15 @@
       <c r="B34" s="3">
         <v>35814.87890625</v>
       </c>
-      <c r="C34" s="3">
+      <c r="C34" s="2"/>
+      <c r="D34" s="3">
         <v>0.12251967731238984</v>
       </c>
-      <c r="D34" s="3">
+      <c r="E34" s="3">
         <v>0.143562963658383</v>
       </c>
-      <c r="E34" s="2"/>
       <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="3">
@@ -964,14 +1021,15 @@
       <c r="B35" s="3">
         <v>36251.85546875</v>
       </c>
-      <c r="C35" s="3">
+      <c r="C35" s="2"/>
+      <c r="D35" s="3">
         <v>0.125929910837945</v>
       </c>
-      <c r="D35" s="3">
+      <c r="E35" s="3">
         <v>0.139039748206838</v>
       </c>
-      <c r="E35" s="2"/>
       <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="3">
@@ -980,14 +1038,15 @@
       <c r="B36" s="3">
         <v>35832.72265625</v>
       </c>
-      <c r="C36" s="3">
+      <c r="C36" s="2"/>
+      <c r="D36" s="3">
         <v>0.13251525064848307</v>
       </c>
-      <c r="D36" s="3">
+      <c r="E36" s="3">
         <v>0.153050156957521</v>
       </c>
-      <c r="E36" s="2"/>
       <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="3">
@@ -996,14 +1055,15 @@
       <c r="B37" s="3">
         <v>36009.90625</v>
       </c>
-      <c r="C37" s="3">
+      <c r="C37" s="2"/>
+      <c r="D37" s="3">
         <v>0.13961989437539993</v>
       </c>
-      <c r="D37" s="3">
+      <c r="E37" s="3">
         <v>0.157155203524274</v>
       </c>
-      <c r="E37" s="2"/>
       <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="3">
@@ -1012,14 +1072,15 @@
       <c r="B38" s="3">
         <v>35818.28515625</v>
       </c>
-      <c r="C38" s="3">
+      <c r="C38" s="2"/>
+      <c r="D38" s="3">
         <v>0.14946589939668775</v>
       </c>
-      <c r="D38" s="3">
+      <c r="E38" s="3">
         <v>0.122275373480069</v>
       </c>
-      <c r="E38" s="2"/>
       <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="3">
@@ -1028,14 +1089,15 @@
       <c r="B39" s="3">
         <v>36035.5</v>
       </c>
-      <c r="C39" s="3">
+      <c r="C39" s="2"/>
+      <c r="D39" s="3">
         <v>0.17010672850115433</v>
       </c>
-      <c r="D39" s="3">
+      <c r="E39" s="3">
         <v>0.148553295605485</v>
       </c>
-      <c r="E39" s="2"/>
       <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="3">
@@ -1044,14 +1106,15 @@
       <c r="B40" s="3">
         <v>35972.46875</v>
       </c>
-      <c r="C40" s="3">
+      <c r="C40" s="2"/>
+      <c r="D40" s="3">
         <v>0.1791822247341874</v>
       </c>
-      <c r="D40" s="3">
+      <c r="E40" s="3">
         <v>0.127175586373652</v>
       </c>
-      <c r="E40" s="2"/>
       <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="3">
@@ -1060,14 +1123,15 @@
       <c r="B41" s="3">
         <v>35860.8515625</v>
       </c>
-      <c r="C41" s="3">
+      <c r="C41" s="2"/>
+      <c r="D41" s="3">
         <v>0.19986132632792059</v>
       </c>
-      <c r="D41" s="3">
+      <c r="E41" s="3">
         <v>0.156619631112655</v>
       </c>
-      <c r="E41" s="2"/>
       <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
       <c r="A42" s="3">
@@ -1076,14 +1140,15 @@
       <c r="B42" s="3">
         <v>35731.99609375</v>
       </c>
-      <c r="C42" s="3">
+      <c r="C42" s="2"/>
+      <c r="D42" s="3">
         <v>0.20514086713521312</v>
       </c>
-      <c r="D42" s="3">
+      <c r="E42" s="3">
         <v>0.180317635209911</v>
       </c>
-      <c r="E42" s="2"/>
       <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
       <c r="A43" s="3">
@@ -1092,14 +1157,15 @@
       <c r="B43" s="3">
         <v>36131.39453125</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43" s="2"/>
+      <c r="D43" s="3">
         <v>0.1815427138638209</v>
       </c>
-      <c r="D43" s="3">
+      <c r="E43" s="3">
         <v>0.164513906770874</v>
       </c>
-      <c r="E43" s="2"/>
       <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="3">
@@ -1108,14 +1174,15 @@
       <c r="B44" s="3">
         <v>35865.1640625</v>
       </c>
-      <c r="C44" s="3">
+      <c r="C44" s="2"/>
+      <c r="D44" s="3">
         <v>0.16149776154211093</v>
       </c>
-      <c r="D44" s="3">
+      <c r="E44" s="3">
         <v>0.155235593806809</v>
       </c>
-      <c r="E44" s="2"/>
       <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="3">
@@ -1124,14 +1191,15 @@
       <c r="B45" s="3">
         <v>35850.88671875</v>
       </c>
-      <c r="C45" s="3">
+      <c r="C45" s="2"/>
+      <c r="D45" s="3">
         <v>0.15146782969031758</v>
       </c>
-      <c r="D45" s="3">
+      <c r="E45" s="3">
         <v>0.16195920694369</v>
       </c>
-      <c r="E45" s="2"/>
       <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
       <c r="A46" s="3">
@@ -1140,14 +1208,15 @@
       <c r="B46" s="3">
         <v>35689.51171875</v>
       </c>
-      <c r="C46" s="3">
+      <c r="C46" s="2"/>
+      <c r="D46" s="3">
         <v>0.13916041429283807</v>
       </c>
-      <c r="D46" s="3">
+      <c r="E46" s="3">
         <v>0.163787430450058</v>
       </c>
-      <c r="E46" s="2"/>
       <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
       <c r="A47" s="3">
@@ -1156,14 +1225,15 @@
       <c r="B47" s="3">
         <v>35778.3671875</v>
       </c>
-      <c r="C47" s="3">
+      <c r="C47" s="2"/>
+      <c r="D47" s="3">
         <v>0.1366490462912372</v>
       </c>
-      <c r="D47" s="3">
+      <c r="E47" s="3">
         <v>0.160840242832262</v>
       </c>
-      <c r="E47" s="2"/>
       <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
       <c r="A48" s="3">
@@ -1172,14 +1242,15 @@
       <c r="B48" s="3">
         <v>35705.37109375</v>
       </c>
-      <c r="C48" s="3">
+      <c r="C48" s="2"/>
+      <c r="D48" s="3">
         <v>0.14288568537301033</v>
       </c>
-      <c r="D48" s="3">
+      <c r="E48" s="3">
         <v>0.167389406402935</v>
       </c>
-      <c r="E48" s="2"/>
       <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
       <c r="A49" s="3">
@@ -1188,14 +1259,15 @@
       <c r="B49" s="3">
         <v>35589.03515625</v>
       </c>
-      <c r="C49" s="3">
+      <c r="C49" s="2"/>
+      <c r="D49" s="3">
         <v>0.14332629811417846</v>
       </c>
-      <c r="D49" s="3">
+      <c r="E49" s="3">
         <v>0.178444435840731</v>
       </c>
-      <c r="E49" s="2"/>
       <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
       <c r="A50" s="3">
@@ -1204,14 +1276,15 @@
       <c r="B50" s="3">
         <v>36526.19140625</v>
       </c>
-      <c r="C50" s="3">
+      <c r="C50" s="2"/>
+      <c r="D50" s="3">
         <v>0.1452307156765199</v>
       </c>
-      <c r="D50" s="3">
+      <c r="E50" s="3">
         <v>0.144528025830284</v>
       </c>
-      <c r="E50" s="2"/>
       <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
       <c r="A51" s="3">
@@ -1220,14 +1293,15 @@
       <c r="B51" s="3">
         <v>35829.7421875</v>
       </c>
-      <c r="C51" s="3">
+      <c r="C51" s="2"/>
+      <c r="D51" s="3">
         <v>0.15091055241421936</v>
       </c>
-      <c r="D51" s="3">
+      <c r="E51" s="3">
         <v>0.164474516095577</v>
       </c>
-      <c r="E51" s="2"/>
       <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
       <c r="A52" s="3">
@@ -1236,14 +1310,15 @@
       <c r="B52" s="3">
         <v>36142.4296875</v>
       </c>
-      <c r="C52" s="3">
+      <c r="C52" s="2"/>
+      <c r="D52" s="3">
         <v>0.15471306312700472</v>
       </c>
-      <c r="D52" s="3">
+      <c r="E52" s="3">
         <v>0.151739483198727</v>
       </c>
-      <c r="E52" s="2"/>
       <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
       <c r="A53" s="3">
@@ -1252,14 +1327,15 @@
       <c r="B53" s="3">
         <v>36263.19140625</v>
       </c>
-      <c r="C53" s="3">
+      <c r="C53" s="2"/>
+      <c r="D53" s="3">
         <v>0.15103514693355205</v>
       </c>
-      <c r="D53" s="3">
+      <c r="E53" s="3">
         <v>0.168540638480872</v>
       </c>
-      <c r="E53" s="2"/>
       <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
       <c r="A54" s="3">
@@ -1268,14 +1344,15 @@
       <c r="B54" s="3">
         <v>35831.15234375</v>
       </c>
-      <c r="C54" s="3">
+      <c r="C54" s="2"/>
+      <c r="D54" s="3">
         <v>0.17696274534150908</v>
       </c>
-      <c r="D54" s="3">
+      <c r="E54" s="3">
         <v>0.189162033883554</v>
       </c>
-      <c r="E54" s="2"/>
       <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
       <c r="A55" s="3">
@@ -1284,14 +1361,15 @@
       <c r="B55" s="3">
         <v>36019.58984375</v>
       </c>
-      <c r="C55" s="3">
+      <c r="C55" s="2"/>
+      <c r="D55" s="3">
         <v>0.17468204347261468</v>
       </c>
-      <c r="D55" s="3">
+      <c r="E55" s="3">
         <v>0.174522369067521</v>
       </c>
-      <c r="E55" s="2"/>
       <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
       <c r="A56" s="3">
@@ -1300,14 +1378,15 @@
       <c r="B56" s="3">
         <v>36118.953125</v>
       </c>
-      <c r="C56" s="3">
+      <c r="C56" s="2"/>
+      <c r="D56" s="3">
         <v>0.16106113996035126</v>
       </c>
-      <c r="D56" s="3">
+      <c r="E56" s="3">
         <v>0.170580680405823</v>
       </c>
-      <c r="E56" s="2"/>
       <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
       <c r="A57" s="3">
@@ -1316,14 +1395,15 @@
       <c r="B57" s="3">
         <v>35318.296875</v>
       </c>
-      <c r="C57" s="3">
+      <c r="C57" s="2"/>
+      <c r="D57" s="3">
         <v>0.15336040502955128</v>
       </c>
-      <c r="D57" s="3">
+      <c r="E57" s="3">
         <v>0.178123320462991</v>
       </c>
-      <c r="E57" s="2"/>
       <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
       <c r="A58" s="3">
@@ -1332,14 +1412,15 @@
       <c r="B58" s="3">
         <v>35721.3203125</v>
       </c>
-      <c r="C58" s="3">
+      <c r="C58" s="2"/>
+      <c r="D58" s="3">
         <v>0.152855882322844</v>
       </c>
-      <c r="D58" s="3">
+      <c r="E58" s="3">
         <v>0.177157696227536</v>
       </c>
-      <c r="E58" s="2"/>
       <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
       <c r="A59" s="3">
@@ -1348,14 +1429,15 @@
       <c r="B59" s="3">
         <v>36487.53515625</v>
       </c>
-      <c r="C59" s="3">
+      <c r="C59" s="2"/>
+      <c r="D59" s="3">
         <v>0.15289137669643035</v>
       </c>
-      <c r="D59" s="3">
+      <c r="E59" s="3">
         <v>0.167250341958252</v>
       </c>
-      <c r="E59" s="2"/>
       <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
       <c r="A60" s="3">
@@ -1364,14 +1446,15 @@
       <c r="B60" s="3">
         <v>36059.046875</v>
       </c>
-      <c r="C60" s="3">
+      <c r="C60" s="2"/>
+      <c r="D60" s="3">
         <v>0.1500814621730204</v>
       </c>
-      <c r="D60" s="3">
+      <c r="E60" s="3">
         <v>0.175734500862807</v>
       </c>
-      <c r="E60" s="2"/>
       <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
       <c r="A61" s="3">
@@ -1380,14 +1463,15 @@
       <c r="B61" s="3">
         <v>36373.953125</v>
       </c>
-      <c r="C61" s="3">
+      <c r="C61" s="2"/>
+      <c r="D61" s="3">
         <v>0.1533150824496947</v>
       </c>
-      <c r="D61" s="3">
+      <c r="E61" s="3">
         <v>0.180641437832458</v>
       </c>
-      <c r="E61" s="2"/>
       <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
       <c r="A62" s="3">
@@ -1396,14 +1480,15 @@
       <c r="B62" s="3">
         <v>35797.3046875</v>
       </c>
-      <c r="C62" s="3">
+      <c r="C62" s="2"/>
+      <c r="D62" s="3">
         <v>0.16433675550192306</v>
       </c>
-      <c r="D62" s="3">
+      <c r="E62" s="3">
         <v>0.160953168678985</v>
       </c>
-      <c r="E62" s="2"/>
       <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
       <c r="A63" s="3">
@@ -1412,14 +1497,15 @@
       <c r="B63" s="3">
         <v>35941.54296875</v>
       </c>
-      <c r="C63" s="3">
+      <c r="C63" s="2"/>
+      <c r="D63" s="3">
         <v>0.20870697446237113</v>
       </c>
-      <c r="D63" s="3">
+      <c r="E63" s="3">
         <v>0.181353046663803</v>
       </c>
-      <c r="E63" s="2"/>
       <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
       <c r="A64" s="3">
@@ -1428,14 +1514,15 @@
       <c r="B64" s="3">
         <v>35616.37890625</v>
       </c>
-      <c r="C64" s="3">
+      <c r="C64" s="2"/>
+      <c r="D64" s="3">
         <v>0.23738929540706785</v>
       </c>
-      <c r="D64" s="3">
+      <c r="E64" s="3">
         <v>0.168878192970217</v>
       </c>
-      <c r="E64" s="2"/>
       <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
       <c r="A65" s="3">
@@ -1444,14 +1531,15 @@
       <c r="B65" s="3">
         <v>36073.1484375</v>
       </c>
-      <c r="C65" s="3">
+      <c r="C65" s="2"/>
+      <c r="D65" s="3">
         <v>0.22942129917586657</v>
       </c>
-      <c r="D65" s="3">
+      <c r="E65" s="3">
         <v>0.185582583343385</v>
       </c>
-      <c r="E65" s="2"/>
       <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
       <c r="A66" s="3">
@@ -1460,14 +1548,15 @@
       <c r="B66" s="3">
         <v>36467.9921875</v>
       </c>
-      <c r="C66" s="3">
+      <c r="C66" s="2"/>
+      <c r="D66" s="3">
         <v>0.22722554040529594</v>
       </c>
-      <c r="D66" s="3">
+      <c r="E66" s="3">
         <v>0.194509361955275</v>
       </c>
-      <c r="E66" s="2"/>
       <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
       <c r="A67" s="3">
@@ -1476,14 +1565,15 @@
       <c r="B67" s="3">
         <v>36007.796875</v>
       </c>
-      <c r="C67" s="3">
+      <c r="C67" s="2"/>
+      <c r="D67" s="3">
         <v>0.19587495849685124</v>
       </c>
-      <c r="D67" s="3">
+      <c r="E67" s="3">
         <v>0.186291675834388</v>
       </c>
-      <c r="E67" s="2"/>
       <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
       <c r="A68" s="3">
@@ -1492,14 +1582,15 @@
       <c r="B68" s="3">
         <v>35854.7265625</v>
       </c>
-      <c r="C68" s="3">
+      <c r="C68" s="2"/>
+      <c r="D68" s="3">
         <v>0.24423325700870116</v>
       </c>
-      <c r="D68" s="3">
+      <c r="E68" s="3">
         <v>0.181470459495236</v>
       </c>
-      <c r="E68" s="2"/>
       <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
       <c r="A69" s="3">
@@ -1508,14 +1599,15 @@
       <c r="B69" s="3">
         <v>35923.30859375</v>
       </c>
-      <c r="C69" s="3">
+      <c r="C69" s="2"/>
+      <c r="D69" s="3">
         <v>0.25067791478303847</v>
       </c>
-      <c r="D69" s="3">
+      <c r="E69" s="3">
         <v>0.189803039608318</v>
       </c>
-      <c r="E69" s="2"/>
       <c r="F69" s="2"/>
+      <c r="G69" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
       <c r="A70" s="3">
@@ -1524,14 +1616,15 @@
       <c r="B70" s="3">
         <v>35729.23828125</v>
       </c>
-      <c r="C70" s="3">
+      <c r="C70" s="2"/>
+      <c r="D70" s="3">
         <v>0.21776803575630763</v>
       </c>
-      <c r="D70" s="3">
+      <c r="E70" s="3">
         <v>0.207082807970914</v>
       </c>
-      <c r="E70" s="2"/>
       <c r="F70" s="2"/>
+      <c r="G70" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
       <c r="A71" s="3">
@@ -1540,14 +1633,15 @@
       <c r="B71" s="3">
         <v>35776.28125</v>
       </c>
-      <c r="C71" s="3">
+      <c r="C71" s="2"/>
+      <c r="D71" s="3">
         <v>0.2046694124649567</v>
       </c>
-      <c r="D71" s="3">
+      <c r="E71" s="3">
         <v>0.217034172414047</v>
       </c>
-      <c r="E71" s="2"/>
       <c r="F71" s="2"/>
+      <c r="G71" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
       <c r="A72" s="3">
@@ -1556,14 +1650,15 @@
       <c r="B72" s="3">
         <v>36390.3046875</v>
       </c>
-      <c r="C72" s="3">
+      <c r="C72" s="2"/>
+      <c r="D72" s="3">
         <v>0.21401777393880184</v>
       </c>
-      <c r="D72" s="3">
+      <c r="E72" s="3">
         <v>0.155103938371166</v>
       </c>
-      <c r="E72" s="2"/>
       <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
       <c r="A73" s="3">
@@ -1572,14 +1667,15 @@
       <c r="B73" s="3">
         <v>36106.890625</v>
       </c>
-      <c r="C73" s="3">
+      <c r="C73" s="2"/>
+      <c r="D73" s="3">
         <v>0.20677446605902025</v>
       </c>
-      <c r="D73" s="3">
+      <c r="E73" s="3">
         <v>0.194921668047142</v>
       </c>
-      <c r="E73" s="2"/>
       <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
       <c r="A74" s="3">
@@ -1588,14 +1684,15 @@
       <c r="B74" s="3">
         <v>35721.625</v>
       </c>
-      <c r="C74" s="3">
+      <c r="C74" s="2"/>
+      <c r="D74" s="3">
         <v>0.1869190730630688</v>
       </c>
-      <c r="D74" s="3">
+      <c r="E74" s="3">
         <v>0.172414736387386</v>
       </c>
-      <c r="E74" s="2"/>
       <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
       <c r="A75" s="3">
@@ -1604,14 +1701,15 @@
       <c r="B75" s="3">
         <v>36034.8125</v>
       </c>
-      <c r="C75" s="3">
+      <c r="C75" s="2"/>
+      <c r="D75" s="3">
         <v>0.17805850816149352</v>
       </c>
-      <c r="D75" s="3">
+      <c r="E75" s="3">
         <v>0.212394354818207</v>
       </c>
-      <c r="E75" s="2"/>
       <c r="F75" s="2"/>
+      <c r="G75" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
       <c r="A76" s="3">
@@ -1620,14 +1718,15 @@
       <c r="B76" s="3">
         <v>36414.1171875</v>
       </c>
-      <c r="C76" s="3">
+      <c r="C76" s="2"/>
+      <c r="D76" s="3">
         <v>0.17704609137102637</v>
       </c>
-      <c r="D76" s="3">
+      <c r="E76" s="3">
         <v>0.245750472450251</v>
       </c>
-      <c r="E76" s="2"/>
       <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
       <c r="A77" s="3">
@@ -1636,14 +1735,15 @@
       <c r="B77" s="3">
         <v>36223.01953125</v>
       </c>
-      <c r="C77" s="3">
+      <c r="C77" s="2"/>
+      <c r="D77" s="3">
         <v>0.1954194546334423</v>
       </c>
-      <c r="D77" s="3">
+      <c r="E77" s="3">
         <v>0.216011677551272</v>
       </c>
-      <c r="E77" s="2"/>
       <c r="F77" s="2"/>
+      <c r="G77" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
       <c r="A78" s="3">
@@ -1652,14 +1752,15 @@
       <c r="B78" s="3">
         <v>35803.3828125</v>
       </c>
-      <c r="C78" s="3">
+      <c r="C78" s="2"/>
+      <c r="D78" s="3">
         <v>0.19857828245033968</v>
       </c>
-      <c r="D78" s="3">
+      <c r="E78" s="3">
         <v>0.204837841860602</v>
       </c>
-      <c r="E78" s="2"/>
       <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
       <c r="A79" s="3">
@@ -1668,14 +1769,15 @@
       <c r="B79" s="3">
         <v>36148.046875</v>
       </c>
-      <c r="C79" s="3">
+      <c r="C79" s="2"/>
+      <c r="D79" s="3">
         <v>0.20092729102417559</v>
       </c>
-      <c r="D79" s="3">
+      <c r="E79" s="3">
         <v>0.21345479604577</v>
       </c>
-      <c r="E79" s="2"/>
       <c r="F79" s="2"/>
+      <c r="G79" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
       <c r="A80" s="3">
@@ -1684,14 +1786,15 @@
       <c r="B80" s="3">
         <v>36230.890625</v>
       </c>
-      <c r="C80" s="3">
+      <c r="C80" s="2"/>
+      <c r="D80" s="3">
         <v>0.20483629135541903</v>
       </c>
-      <c r="D80" s="3">
+      <c r="E80" s="3">
         <v>0.221225163638852</v>
       </c>
-      <c r="E80" s="2"/>
       <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
       <c r="A81" s="3">
@@ -1700,14 +1803,15 @@
       <c r="B81" s="3">
         <v>35756.64453125</v>
       </c>
-      <c r="C81" s="3">
+      <c r="C81" s="2"/>
+      <c r="D81" s="3">
         <v>0.21379777715826148</v>
       </c>
-      <c r="D81" s="3">
+      <c r="E81" s="3">
         <v>0.225019443773977</v>
       </c>
-      <c r="E81" s="2"/>
       <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
       <c r="A82" s="3">
@@ -1716,14 +1820,15 @@
       <c r="B82" s="3">
         <v>36058.03125</v>
       </c>
-      <c r="C82" s="3">
+      <c r="C82" s="2"/>
+      <c r="D82" s="3">
         <v>0.2292939342671418</v>
       </c>
-      <c r="D82" s="3">
+      <c r="E82" s="3">
         <v>0.198447271648623</v>
       </c>
-      <c r="E82" s="2"/>
       <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
       <c r="A83" s="3">
@@ -1732,14 +1837,15 @@
       <c r="B83" s="3">
         <v>36354.9453125</v>
       </c>
-      <c r="C83" s="3">
+      <c r="C83" s="2"/>
+      <c r="D83" s="3">
         <v>0.24660782617233057</v>
       </c>
-      <c r="D83" s="3">
+      <c r="E83" s="3">
         <v>0.219364117119579</v>
       </c>
-      <c r="E83" s="2"/>
       <c r="F83" s="2"/>
+      <c r="G83" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
       <c r="A84" s="3">
@@ -1748,14 +1854,15 @@
       <c r="B84" s="3">
         <v>36248.68359375</v>
       </c>
-      <c r="C84" s="3">
+      <c r="C84" s="2"/>
+      <c r="D84" s="3">
         <v>0.2669391369202328</v>
       </c>
-      <c r="D84" s="3">
+      <c r="E84" s="3">
         <v>0.204307274031018</v>
       </c>
-      <c r="E84" s="2"/>
       <c r="F84" s="2"/>
+      <c r="G84" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
       <c r="A85" s="3">
@@ -1764,14 +1871,15 @@
       <c r="B85" s="3">
         <v>35885.38671875</v>
       </c>
-      <c r="C85" s="3">
+      <c r="C85" s="2"/>
+      <c r="D85" s="3">
         <v>0.28192679865762016</v>
       </c>
-      <c r="D85" s="3">
+      <c r="E85" s="3">
         <v>0.223604178487923</v>
       </c>
-      <c r="E85" s="2"/>
       <c r="F85" s="2"/>
+      <c r="G85" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
       <c r="A86" s="3">
@@ -1780,14 +1888,15 @@
       <c r="B86" s="3">
         <v>36561.078125</v>
       </c>
-      <c r="C86" s="3">
+      <c r="C86" s="2"/>
+      <c r="D86" s="3">
         <v>0.27924295291016016</v>
       </c>
-      <c r="D86" s="3">
+      <c r="E86" s="3">
         <v>0.238979432250454</v>
       </c>
-      <c r="E86" s="2"/>
       <c r="F86" s="2"/>
+      <c r="G86" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
       <c r="A87" s="3">
@@ -1796,14 +1905,15 @@
       <c r="B87" s="3">
         <v>36180.8359375</v>
       </c>
-      <c r="C87" s="3">
+      <c r="C87" s="2"/>
+      <c r="D87" s="3">
         <v>0.27300911128090644</v>
       </c>
-      <c r="D87" s="3">
+      <c r="E87" s="3">
         <v>0.226084080099344</v>
       </c>
-      <c r="E87" s="2"/>
       <c r="F87" s="2"/>
+      <c r="G87" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
       <c r="A88" s="3">
@@ -1812,14 +1922,15 @@
       <c r="B88" s="3">
         <v>35800.7109375</v>
       </c>
-      <c r="C88" s="3">
+      <c r="C88" s="2"/>
+      <c r="D88" s="3">
         <v>0.26424209449123737</v>
       </c>
-      <c r="D88" s="3">
+      <c r="E88" s="3">
         <v>0.220477497600689</v>
       </c>
-      <c r="E88" s="2"/>
       <c r="F88" s="2"/>
+      <c r="G88" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
       <c r="A89" s="3">
@@ -1828,14 +1939,15 @@
       <c r="B89" s="3">
         <v>35684.1953125</v>
       </c>
-      <c r="C89" s="3">
+      <c r="C89" s="2"/>
+      <c r="D89" s="3">
         <v>0.24197602301875518</v>
       </c>
-      <c r="D89" s="3">
+      <c r="E89" s="3">
         <v>0.225928530821089</v>
       </c>
-      <c r="E89" s="2"/>
       <c r="F89" s="2"/>
+      <c r="G89" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
       <c r="A90" s="3">
@@ -1844,14 +1956,15 @@
       <c r="B90" s="3">
         <v>35930.2578125</v>
       </c>
-      <c r="C90" s="3">
+      <c r="C90" s="2"/>
+      <c r="D90" s="3">
         <v>0.2419944885276304</v>
       </c>
-      <c r="D90" s="3">
+      <c r="E90" s="3">
         <v>0.230364124297231</v>
       </c>
-      <c r="E90" s="2"/>
       <c r="F90" s="2"/>
+      <c r="G90" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
       <c r="A91" s="3">
@@ -1860,14 +1973,15 @@
       <c r="B91" s="3">
         <v>35647.49609375</v>
       </c>
-      <c r="C91" s="3">
+      <c r="C91" s="2"/>
+      <c r="D91" s="3">
         <v>0.25547378715464486</v>
       </c>
-      <c r="D91" s="3">
+      <c r="E91" s="3">
         <v>0.227890864224224</v>
       </c>
-      <c r="E91" s="2"/>
       <c r="F91" s="2"/>
+      <c r="G91" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
       <c r="A92" s="3">
@@ -1876,14 +1990,15 @@
       <c r="B92" s="3">
         <v>36177.59765625</v>
       </c>
-      <c r="C92" s="3">
+      <c r="C92" s="2"/>
+      <c r="D92" s="3">
         <v>0.270842502955752</v>
       </c>
-      <c r="D92" s="3">
+      <c r="E92" s="3">
         <v>0.222820523402751</v>
       </c>
-      <c r="E92" s="2"/>
       <c r="F92" s="2"/>
+      <c r="G92" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
       <c r="A93" s="3">
@@ -1892,14 +2007,15 @@
       <c r="B93" s="3">
         <v>36024.875</v>
       </c>
-      <c r="C93" s="3">
+      <c r="C93" s="2"/>
+      <c r="D93" s="3">
         <v>0.28353584767645645</v>
       </c>
-      <c r="D93" s="3">
+      <c r="E93" s="3">
         <v>0.226261088936281</v>
       </c>
-      <c r="E93" s="2"/>
       <c r="F93" s="2"/>
+      <c r="G93" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
       <c r="A94" s="3">
@@ -1908,14 +2024,15 @@
       <c r="B94" s="3">
         <v>36134.22265625</v>
       </c>
-      <c r="C94" s="3">
+      <c r="C94" s="2"/>
+      <c r="D94" s="3">
         <v>0.29463095501639647</v>
       </c>
-      <c r="D94" s="3">
+      <c r="E94" s="3">
         <v>0.224467546754524</v>
       </c>
-      <c r="E94" s="2"/>
       <c r="F94" s="2"/>
+      <c r="G94" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
       <c r="A95" s="3">
@@ -1924,14 +2041,15 @@
       <c r="B95" s="3">
         <v>36043.7578125</v>
       </c>
-      <c r="C95" s="3">
+      <c r="C95" s="2"/>
+      <c r="D95" s="3">
         <v>0.2986756553317926</v>
       </c>
-      <c r="D95" s="3">
+      <c r="E95" s="3">
         <v>0.224684419585064</v>
       </c>
-      <c r="E95" s="2"/>
       <c r="F95" s="2"/>
+      <c r="G95" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
       <c r="A96" s="3">
@@ -1940,14 +2058,15 @@
       <c r="B96" s="3">
         <v>35889.55859375</v>
       </c>
-      <c r="C96" s="3">
+      <c r="C96" s="2"/>
+      <c r="D96" s="3">
         <v>0.28907585485702597</v>
       </c>
-      <c r="D96" s="3">
+      <c r="E96" s="3">
         <v>0.229935901014017</v>
       </c>
-      <c r="E96" s="2"/>
       <c r="F96" s="2"/>
+      <c r="G96" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
       <c r="A97" s="3">
@@ -1956,14 +2075,15 @@
       <c r="B97" s="3">
         <v>35836.375</v>
       </c>
-      <c r="C97" s="3">
+      <c r="C97" s="2"/>
+      <c r="D97" s="3">
         <v>0.2595220378065569</v>
       </c>
-      <c r="D97" s="3">
+      <c r="E97" s="3">
         <v>0.227902591812446</v>
       </c>
-      <c r="E97" s="2"/>
       <c r="F97" s="2"/>
+      <c r="G97" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
       <c r="A98" s="3">
@@ -1972,14 +2092,15 @@
       <c r="B98" s="3">
         <v>36097.58984375</v>
       </c>
-      <c r="C98" s="3">
+      <c r="C98" s="2"/>
+      <c r="D98" s="3">
         <v>0.237515423315677</v>
       </c>
-      <c r="D98" s="3">
+      <c r="E98" s="3">
         <v>0.227147145623394</v>
       </c>
-      <c r="E98" s="2"/>
       <c r="F98" s="2"/>
+      <c r="G98" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
       <c r="A99" s="3">
@@ -1988,14 +2109,15 @@
       <c r="B99" s="3">
         <v>35841.7109375</v>
       </c>
-      <c r="C99" s="3">
+      <c r="C99" s="2"/>
+      <c r="D99" s="3">
         <v>0.22532808305420313</v>
       </c>
-      <c r="D99" s="3">
+      <c r="E99" s="3">
         <v>0.225595871480371</v>
       </c>
-      <c r="E99" s="2"/>
       <c r="F99" s="2"/>
+      <c r="G99" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
       <c r="A100" s="3">
@@ -2004,14 +2126,15 @@
       <c r="B100" s="3">
         <v>35930.98828125</v>
       </c>
-      <c r="C100" s="3">
+      <c r="C100" s="2"/>
+      <c r="D100" s="3">
         <v>0.22145728682665644</v>
       </c>
-      <c r="D100" s="3">
+      <c r="E100" s="3">
         <v>0.22707342538249</v>
       </c>
-      <c r="E100" s="2"/>
       <c r="F100" s="2"/>
+      <c r="G100" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
       <c r="A101" s="3">
@@ -2020,14 +2143,15 @@
       <c r="B101" s="3">
         <v>36671.015625</v>
       </c>
-      <c r="C101" s="3">
+      <c r="C101" s="2"/>
+      <c r="D101" s="3">
         <v>0.22293851410800772</v>
       </c>
-      <c r="D101" s="3">
+      <c r="E101" s="3">
         <v>0.2216044310955</v>
       </c>
-      <c r="E101" s="2"/>
       <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
       <c r="A102" s="3">
@@ -2036,14 +2160,15 @@
       <c r="B102" s="3">
         <v>35850.05078125</v>
       </c>
-      <c r="C102" s="3">
+      <c r="C102" s="2"/>
+      <c r="D102" s="3">
         <v>0.23477965349063243</v>
       </c>
-      <c r="D102" s="3">
+      <c r="E102" s="3">
         <v>0.224863132261657</v>
       </c>
-      <c r="E102" s="2"/>
       <c r="F102" s="2"/>
+      <c r="G102" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
       <c r="A103" s="3">
@@ -2052,14 +2177,15 @@
       <c r="B103" s="3">
         <v>35948.09375</v>
       </c>
-      <c r="C103" s="3">
+      <c r="C103" s="2"/>
+      <c r="D103" s="3">
         <v>0.2437493788730145</v>
       </c>
-      <c r="D103" s="3">
+      <c r="E103" s="3">
         <v>0.225352117209522</v>
       </c>
-      <c r="E103" s="2"/>
       <c r="F103" s="2"/>
+      <c r="G103" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
       <c r="A104" s="3">
@@ -2068,14 +2194,15 @@
       <c r="B104" s="3">
         <v>35814.2265625</v>
       </c>
-      <c r="C104" s="3">
+      <c r="C104" s="2"/>
+      <c r="D104" s="3">
         <v>0.25904797152940046</v>
       </c>
-      <c r="D104" s="3">
+      <c r="E104" s="3">
         <v>0.228025407874481</v>
       </c>
-      <c r="E104" s="2"/>
       <c r="F104" s="2"/>
+      <c r="G104" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
       <c r="A105" s="3">
@@ -2084,14 +2211,15 @@
       <c r="B105" s="3">
         <v>35676.625</v>
       </c>
-      <c r="C105" s="3">
+      <c r="C105" s="2"/>
+      <c r="D105" s="3">
         <v>0.26633887795654576</v>
       </c>
-      <c r="D105" s="3">
+      <c r="E105" s="3">
         <v>0.231813686034845</v>
       </c>
-      <c r="E105" s="2"/>
       <c r="F105" s="2"/>
+      <c r="G105" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75">
       <c r="A106" s="3">
@@ -2100,14 +2228,15 @@
       <c r="B106" s="3">
         <v>35974.3046875</v>
       </c>
-      <c r="C106" s="3">
+      <c r="C106" s="2"/>
+      <c r="D106" s="3">
         <v>0.2537763146393246</v>
       </c>
-      <c r="D106" s="3">
+      <c r="E106" s="3">
         <v>0.225619923934059</v>
       </c>
-      <c r="E106" s="2"/>
       <c r="F106" s="2"/>
+      <c r="G106" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
       <c r="A107" s="3">
@@ -2116,14 +2245,15 @@
       <c r="B107" s="3">
         <v>35930.4609375</v>
       </c>
-      <c r="C107" s="3">
+      <c r="C107" s="2"/>
+      <c r="D107" s="3">
         <v>0.23095593888676652</v>
       </c>
-      <c r="D107" s="3">
+      <c r="E107" s="3">
         <v>0.228670728557505</v>
       </c>
-      <c r="E107" s="2"/>
       <c r="F107" s="2"/>
+      <c r="G107" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
       <c r="A108" s="3">
@@ -2132,14 +2262,15 @@
       <c r="B108" s="3">
         <v>36690.8984375</v>
       </c>
-      <c r="C108" s="3">
+      <c r="C108" s="2"/>
+      <c r="D108" s="3">
         <v>0.21347625663542427</v>
       </c>
-      <c r="D108" s="3">
+      <c r="E108" s="3">
         <v>0.219596048190268</v>
       </c>
-      <c r="E108" s="2"/>
       <c r="F108" s="2"/>
+      <c r="G108" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75">
       <c r="A109" s="3">
@@ -2148,14 +2279,15 @@
       <c r="B109" s="3">
         <v>35653.27734375</v>
       </c>
-      <c r="C109" s="3">
+      <c r="C109" s="2"/>
+      <c r="D109" s="3">
         <v>0.20272033161792483</v>
       </c>
-      <c r="D109" s="3">
+      <c r="E109" s="3">
         <v>0.224944504374396</v>
       </c>
-      <c r="E109" s="2"/>
       <c r="F109" s="2"/>
+      <c r="G109" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75">
       <c r="A110" s="3">
@@ -2164,14 +2296,15 @@
       <c r="B110" s="3">
         <v>35939.6484375</v>
       </c>
-      <c r="C110" s="3">
+      <c r="C110" s="2"/>
+      <c r="D110" s="3">
         <v>0.20290635797941964</v>
       </c>
-      <c r="D110" s="3">
+      <c r="E110" s="3">
         <v>0.227953364233928</v>
       </c>
-      <c r="E110" s="2"/>
       <c r="F110" s="2"/>
+      <c r="G110" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75">
       <c r="A111" s="3">
@@ -2180,14 +2313,15 @@
       <c r="B111" s="3">
         <v>37807.08203125</v>
       </c>
-      <c r="C111" s="3">
+      <c r="C111" s="2"/>
+      <c r="D111" s="3">
         <v>0.20905754196425952</v>
       </c>
-      <c r="D111" s="3">
+      <c r="E111" s="3">
         <v>0.213759862943698</v>
       </c>
-      <c r="E111" s="2"/>
       <c r="F111" s="2"/>
+      <c r="G111" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75">
       <c r="A112" s="3">
@@ -2196,14 +2330,15 @@
       <c r="B112" s="3">
         <v>48912.5625</v>
       </c>
-      <c r="C112" s="3">
+      <c r="C112" s="2"/>
+      <c r="D112" s="3">
         <v>0.24557366318849755</v>
       </c>
-      <c r="D112" s="3">
+      <c r="E112" s="3">
         <v>0.179155635368948</v>
       </c>
-      <c r="E112" s="2"/>
       <c r="F112" s="2"/>
+      <c r="G112" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75">
       <c r="A113" s="3">
@@ -2212,14 +2347,15 @@
       <c r="B113" s="3">
         <v>42272.22265625</v>
       </c>
-      <c r="C113" s="3">
+      <c r="C113" s="2"/>
+      <c r="D113" s="3">
         <v>0.2686161427830586</v>
       </c>
-      <c r="D113" s="3">
+      <c r="E113" s="3">
         <v>0.202444364480205</v>
       </c>
-      <c r="E113" s="2"/>
       <c r="F113" s="2"/>
+      <c r="G113" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75">
       <c r="A114" s="3">
@@ -2228,14 +2364,15 @@
       <c r="B114" s="3">
         <v>43092.41796875</v>
       </c>
-      <c r="C114" s="3">
+      <c r="C114" s="2"/>
+      <c r="D114" s="3">
         <v>0.3163232283502813</v>
       </c>
-      <c r="D114" s="3">
+      <c r="E114" s="3">
         <v>0.241725737470278</v>
       </c>
-      <c r="E114" s="2"/>
       <c r="F114" s="2"/>
+      <c r="G114" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18.75">
       <c r="A115" s="3">
@@ -2244,14 +2381,15 @@
       <c r="B115" s="3">
         <v>44012.40234375</v>
       </c>
-      <c r="C115" s="3">
+      <c r="C115" s="2"/>
+      <c r="D115" s="3">
         <v>0.3264104576728035</v>
       </c>
-      <c r="D115" s="3">
+      <c r="E115" s="3">
         <v>0.240689444833084</v>
       </c>
-      <c r="E115" s="2"/>
       <c r="F115" s="2"/>
+      <c r="G115" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18.75">
       <c r="A116" s="3">
@@ -2260,14 +2398,15 @@
       <c r="B116" s="3">
         <v>43110.22265625</v>
       </c>
-      <c r="C116" s="3">
+      <c r="C116" s="2"/>
+      <c r="D116" s="3">
         <v>0.29663488493946943</v>
       </c>
-      <c r="D116" s="3">
+      <c r="E116" s="3">
         <v>0.30148827369082</v>
       </c>
-      <c r="E116" s="2"/>
       <c r="F116" s="2"/>
+      <c r="G116" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18.75">
       <c r="A117" s="3">
@@ -2276,14 +2415,15 @@
       <c r="B117" s="3">
         <v>43765.59765625</v>
       </c>
-      <c r="C117" s="3">
+      <c r="C117" s="2"/>
+      <c r="D117" s="3">
         <v>0.2774135489863548</v>
       </c>
-      <c r="D117" s="3">
+      <c r="E117" s="3">
         <v>0.238191336445375</v>
       </c>
-      <c r="E117" s="2"/>
       <c r="F117" s="2"/>
+      <c r="G117" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18.75">
       <c r="A118" s="3">
@@ -2292,14 +2432,15 @@
       <c r="B118" s="3">
         <v>43121.93359375</v>
       </c>
-      <c r="C118" s="3">
+      <c r="C118" s="2"/>
+      <c r="D118" s="3">
         <v>0.26604419420615993</v>
       </c>
-      <c r="D118" s="3">
+      <c r="E118" s="3">
         <v>0.216569019958502</v>
       </c>
-      <c r="E118" s="2"/>
       <c r="F118" s="2"/>
+      <c r="G118" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18.75">
       <c r="A119" s="3">
@@ -2308,14 +2449,15 @@
       <c r="B119" s="3">
         <v>43699.859375</v>
       </c>
-      <c r="C119" s="3">
+      <c r="C119" s="2"/>
+      <c r="D119" s="3">
         <v>0.25950988097921074</v>
       </c>
-      <c r="D119" s="3">
+      <c r="E119" s="3">
         <v>0.24108359828845</v>
       </c>
-      <c r="E119" s="2"/>
       <c r="F119" s="2"/>
+      <c r="G119" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18.75">
       <c r="A120" s="3">
@@ -2324,14 +2466,15 @@
       <c r="B120" s="3">
         <v>43235.515625</v>
       </c>
-      <c r="C120" s="3">
+      <c r="C120" s="2"/>
+      <c r="D120" s="3">
         <v>0.25832381133491644</v>
       </c>
-      <c r="D120" s="3">
+      <c r="E120" s="3">
         <v>0.235090390369719</v>
       </c>
-      <c r="E120" s="2"/>
       <c r="F120" s="2"/>
+      <c r="G120" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18.75">
       <c r="A121" s="3">
@@ -2340,14 +2483,15 @@
       <c r="B121" s="3">
         <v>43473.73046875</v>
       </c>
-      <c r="C121" s="3">
+      <c r="C121" s="2"/>
+      <c r="D121" s="3">
         <v>0.24762128513143886</v>
       </c>
-      <c r="D121" s="3">
+      <c r="E121" s="3">
         <v>0.220449554918856</v>
       </c>
-      <c r="E121" s="2"/>
       <c r="F121" s="2"/>
+      <c r="G121" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18.75">
       <c r="A122" s="3">
@@ -2356,14 +2500,15 @@
       <c r="B122" s="3">
         <v>43507.953125</v>
       </c>
-      <c r="C122" s="3">
+      <c r="C122" s="2"/>
+      <c r="D122" s="3">
         <v>0.2546262371810825</v>
       </c>
-      <c r="D122" s="3">
+      <c r="E122" s="3">
         <v>0.245674195285603</v>
       </c>
-      <c r="E122" s="2"/>
       <c r="F122" s="2"/>
+      <c r="G122" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18.75">
       <c r="A123" s="3">
@@ -2372,14 +2517,15 @@
       <c r="B123" s="3">
         <v>43769.71875</v>
       </c>
-      <c r="C123" s="3">
+      <c r="C123" s="2"/>
+      <c r="D123" s="3">
         <v>0.2529113404955147</v>
       </c>
-      <c r="D123" s="3">
+      <c r="E123" s="3">
         <v>0.229096477647045</v>
       </c>
-      <c r="E123" s="2"/>
       <c r="F123" s="2"/>
+      <c r="G123" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75">
       <c r="A124" s="3">
@@ -2388,14 +2534,15 @@
       <c r="B124" s="3">
         <v>39443.5703125</v>
       </c>
-      <c r="C124" s="3">
+      <c r="C124" s="2"/>
+      <c r="D124" s="3">
         <v>0.24682385102841575</v>
       </c>
-      <c r="D124" s="3">
+      <c r="E124" s="3">
         <v>0.226303886460725</v>
       </c>
-      <c r="E124" s="2"/>
       <c r="F124" s="2"/>
+      <c r="G124" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75">
       <c r="A125" s="3">
@@ -2404,14 +2551,15 @@
       <c r="B125" s="3">
         <v>34269.328125</v>
       </c>
-      <c r="C125" s="3">
+      <c r="C125" s="2"/>
+      <c r="D125" s="3">
         <v>0.22659524141167608</v>
       </c>
-      <c r="D125" s="3">
+      <c r="E125" s="3">
         <v>0.198522782687933</v>
       </c>
-      <c r="E125" s="2"/>
       <c r="F125" s="2"/>
+      <c r="G125" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18.75">
       <c r="A126" s="3">
@@ -2420,14 +2568,15 @@
       <c r="B126" s="3">
         <v>35394.41796875</v>
       </c>
-      <c r="C126" s="3">
+      <c r="C126" s="2"/>
+      <c r="D126" s="3">
         <v>0.21285960095727519</v>
       </c>
-      <c r="D126" s="3">
+      <c r="E126" s="3">
         <v>0.229698476208116</v>
       </c>
-      <c r="E126" s="2"/>
       <c r="F126" s="2"/>
+      <c r="G126" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75">
       <c r="A127" s="3">
@@ -2436,14 +2585,15 @@
       <c r="B127" s="3">
         <v>35817.88671875</v>
       </c>
-      <c r="C127" s="3">
+      <c r="C127" s="2"/>
+      <c r="D127" s="3">
         <v>0.19275693964030197</v>
       </c>
-      <c r="D127" s="3">
+      <c r="E127" s="3">
         <v>0.212817441204679</v>
       </c>
-      <c r="E127" s="2"/>
       <c r="F127" s="2"/>
+      <c r="G127" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18.75">
       <c r="A128" s="3">
@@ -2452,14 +2602,15 @@
       <c r="B128" s="3">
         <v>35961.59375</v>
       </c>
-      <c r="C128" s="3">
+      <c r="C128" s="2"/>
+      <c r="D128" s="3">
         <v>0.18026056097981719</v>
       </c>
-      <c r="D128" s="3">
+      <c r="E128" s="3">
         <v>0.200613562015691</v>
       </c>
-      <c r="E128" s="2"/>
       <c r="F128" s="2"/>
+      <c r="G128" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18.75">
       <c r="A129" s="3">
@@ -2468,14 +2619,15 @@
       <c r="B129" s="3">
         <v>36286.69140625</v>
       </c>
-      <c r="C129" s="3">
+      <c r="C129" s="2"/>
+      <c r="D129" s="3">
         <v>0.17390763118397448</v>
       </c>
-      <c r="D129" s="3">
+      <c r="E129" s="3">
         <v>0.194880438850899</v>
       </c>
-      <c r="E129" s="2"/>
       <c r="F129" s="2"/>
+      <c r="G129" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18.75">
       <c r="A130" s="3">
@@ -2484,14 +2636,15 @@
       <c r="B130" s="3">
         <v>36154.19140625</v>
       </c>
-      <c r="C130" s="3">
+      <c r="C130" s="2"/>
+      <c r="D130" s="3">
         <v>0.17541083652282602</v>
       </c>
-      <c r="D130" s="3">
+      <c r="E130" s="3">
         <v>0.20215421449023</v>
       </c>
-      <c r="E130" s="2"/>
       <c r="F130" s="2"/>
+      <c r="G130" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18.75">
       <c r="A131" s="3">
@@ -2500,14 +2653,15 @@
       <c r="B131" s="3">
         <v>45604.8671875</v>
       </c>
-      <c r="C131" s="3">
+      <c r="C131" s="2"/>
+      <c r="D131" s="3">
         <v>0.1815000399341419</v>
       </c>
-      <c r="D131" s="3">
+      <c r="E131" s="3">
         <v>0.173129329279399</v>
       </c>
-      <c r="E131" s="2"/>
       <c r="F131" s="2"/>
+      <c r="G131" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="18.75">
       <c r="A132" s="3">
@@ -2516,14 +2670,15 @@
       <c r="B132" s="3">
         <v>44110.33984375</v>
       </c>
-      <c r="C132" s="3">
+      <c r="C132" s="2"/>
+      <c r="D132" s="3">
         <v>0.18325384860918192</v>
       </c>
-      <c r="D132" s="3">
+      <c r="E132" s="3">
         <v>0.190575458016597</v>
       </c>
-      <c r="E132" s="2"/>
       <c r="F132" s="2"/>
+      <c r="G132" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18.75">
       <c r="A133" s="3">
@@ -2532,14 +2687,15 @@
       <c r="B133" s="3">
         <v>42774.41796875</v>
       </c>
-      <c r="C133" s="3">
+      <c r="C133" s="2"/>
+      <c r="D133" s="3">
         <v>0.1913044671189727</v>
       </c>
-      <c r="D133" s="3">
+      <c r="E133" s="3">
         <v>0.209402960679191</v>
       </c>
-      <c r="E133" s="2"/>
       <c r="F133" s="2"/>
+      <c r="G133" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="18.75">
       <c r="A134" s="3">
@@ -2548,14 +2704,15 @@
       <c r="B134" s="3">
         <v>43974.1875</v>
       </c>
-      <c r="C134" s="3">
+      <c r="C134" s="2"/>
+      <c r="D134" s="3">
         <v>0.20275905330631822</v>
       </c>
-      <c r="D134" s="3">
+      <c r="E134" s="3">
         <v>0.249545640347789</v>
       </c>
-      <c r="E134" s="2"/>
       <c r="F134" s="2"/>
+      <c r="G134" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="18.75">
       <c r="A135" s="3">
@@ -2564,14 +2721,15 @@
       <c r="B135" s="3">
         <v>43362.87109375</v>
       </c>
-      <c r="C135" s="3">
+      <c r="C135" s="2"/>
+      <c r="D135" s="3">
         <v>0.24026074828190444</v>
       </c>
-      <c r="D135" s="3">
+      <c r="E135" s="3">
         <v>0.266395562976848</v>
       </c>
-      <c r="E135" s="2"/>
       <c r="F135" s="2"/>
+      <c r="G135" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75">
       <c r="A136" s="3">
@@ -2580,14 +2738,15 @@
       <c r="B136" s="3">
         <v>43532.83984375</v>
       </c>
-      <c r="C136" s="3">
+      <c r="C136" s="2"/>
+      <c r="D136" s="3">
         <v>0.22806531882104977</v>
       </c>
-      <c r="D136" s="3">
+      <c r="E136" s="3">
         <v>0.278482960552853</v>
       </c>
-      <c r="E136" s="2"/>
       <c r="F136" s="2"/>
+      <c r="G136" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18.75">
       <c r="A137" s="3">
@@ -2596,14 +2755,15 @@
       <c r="B137" s="3">
         <v>43468.20703125</v>
       </c>
-      <c r="C137" s="3">
+      <c r="C137" s="2"/>
+      <c r="D137" s="3">
         <v>0.199420260163303</v>
       </c>
-      <c r="D137" s="3">
+      <c r="E137" s="3">
         <v>0.233940717402472</v>
       </c>
-      <c r="E137" s="2"/>
       <c r="F137" s="2"/>
+      <c r="G137" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="18.75">
       <c r="A138" s="3">
@@ -2612,14 +2772,15 @@
       <c r="B138" s="3">
         <v>43539.81640625</v>
       </c>
-      <c r="C138" s="3">
+      <c r="C138" s="2"/>
+      <c r="D138" s="3">
         <v>0.1768645508423794</v>
       </c>
-      <c r="D138" s="3">
+      <c r="E138" s="3">
         <v>0.242853067805119</v>
       </c>
-      <c r="E138" s="2"/>
       <c r="F138" s="2"/>
+      <c r="G138" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="18.75">
       <c r="A139" s="3">
@@ -2628,14 +2789,15 @@
       <c r="B139" s="3">
         <v>43468.3984375</v>
       </c>
-      <c r="C139" s="3">
+      <c r="C139" s="2"/>
+      <c r="D139" s="3">
         <v>0.1546150556049688</v>
       </c>
-      <c r="D139" s="3">
+      <c r="E139" s="3">
         <v>0.235257879715869</v>
       </c>
-      <c r="E139" s="2"/>
       <c r="F139" s="2"/>
+      <c r="G139" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="18.75">
       <c r="A140" s="3">
@@ -2644,14 +2806,15 @@
       <c r="B140" s="3">
         <v>43293.125</v>
       </c>
-      <c r="C140" s="3">
+      <c r="C140" s="2"/>
+      <c r="D140" s="3">
         <v>0.1417358546840911</v>
       </c>
-      <c r="D140" s="3">
+      <c r="E140" s="3">
         <v>0.218069848068073</v>
       </c>
-      <c r="E140" s="2"/>
       <c r="F140" s="2"/>
+      <c r="G140" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="18.75">
       <c r="A141" s="3">
@@ -2660,14 +2823,15 @@
       <c r="B141" s="3">
         <v>43370.91796875</v>
       </c>
-      <c r="C141" s="3">
+      <c r="C141" s="2"/>
+      <c r="D141" s="3">
         <v>0.12955817095233735</v>
       </c>
-      <c r="D141" s="3">
+      <c r="E141" s="3">
         <v>0.228623103153784</v>
       </c>
-      <c r="E141" s="2"/>
       <c r="F141" s="2"/>
+      <c r="G141" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="18.75">
       <c r="A142" s="3">
@@ -2676,14 +2840,15 @@
       <c r="B142" s="3">
         <v>43492.63671875</v>
       </c>
-      <c r="C142" s="3">
+      <c r="C142" s="2"/>
+      <c r="D142" s="3">
         <v>0.12666271977252058</v>
       </c>
-      <c r="D142" s="3">
+      <c r="E142" s="3">
         <v>0.216695068350596</v>
       </c>
-      <c r="E142" s="2"/>
       <c r="F142" s="2"/>
+      <c r="G142" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="18.75">
       <c r="A143" s="3">
@@ -2692,14 +2857,15 @@
       <c r="B143" s="3">
         <v>43679.77734375</v>
       </c>
-      <c r="C143" s="3">
+      <c r="C143" s="2"/>
+      <c r="D143" s="3">
         <v>0.12244679507601958</v>
       </c>
-      <c r="D143" s="3">
+      <c r="E143" s="3">
         <v>0.227048585584216</v>
       </c>
-      <c r="E143" s="2"/>
       <c r="F143" s="2"/>
+      <c r="G143" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="18.75">
       <c r="A144" s="3">
@@ -2708,14 +2874,15 @@
       <c r="B144" s="3">
         <v>43202.51171875</v>
       </c>
-      <c r="C144" s="3">
+      <c r="C144" s="2"/>
+      <c r="D144" s="3">
         <v>0.12086712667581326</v>
       </c>
-      <c r="D144" s="3">
+      <c r="E144" s="3">
         <v>0.219692759516058</v>
       </c>
-      <c r="E144" s="2"/>
       <c r="F144" s="2"/>
+      <c r="G144" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="18.75">
       <c r="A145" s="3">
@@ -2724,14 +2891,15 @@
       <c r="B145" s="3">
         <v>43816.6484375</v>
       </c>
-      <c r="C145" s="3">
+      <c r="C145" s="2"/>
+      <c r="D145" s="3">
         <v>0.1082928874023353</v>
       </c>
-      <c r="D145" s="3">
+      <c r="E145" s="3">
         <v>0.225007892678546</v>
       </c>
-      <c r="E145" s="2"/>
       <c r="F145" s="2"/>
+      <c r="G145" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>